<commit_message>
Removed the duplicates from the data set
</commit_message>
<xml_diff>
--- a/Bike sales.xlsx
+++ b/Bike sales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshr\Desktop\Data analytics\Excel\Excel-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D37B2A-46E5-49C0-B2DF-0B67056761D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D4013D-9698-4C91-A0DE-157CDC32CBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bike_buyers!$A$1:$M$1001</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Working Sheet'!$A$1:$M$1027</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Working Sheet'!$A$1:$M$1001</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16442" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16234" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -43114,10 +43114,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2CB67A-7E7D-470D-BF7C-52E0887E6CCE}">
-  <dimension ref="A1:M1027"/>
+  <dimension ref="A1:M1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -84166,1074 +84166,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="1002" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1002">
-        <v>13507</v>
-      </c>
-      <c r="B1002" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1002" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1002" s="1">
-        <v>10000</v>
-      </c>
-      <c r="E1002">
-        <v>2</v>
-      </c>
-      <c r="F1002" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1002" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1002" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1002">
-        <v>0</v>
-      </c>
-      <c r="J1002" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1002" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1002">
-        <v>50</v>
-      </c>
-      <c r="M1002" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1003" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1003">
-        <v>19280</v>
-      </c>
-      <c r="B1003" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1003" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1003" s="1">
-        <v>120000</v>
-      </c>
-      <c r="E1003">
-        <v>2</v>
-      </c>
-      <c r="F1003" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1003" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1003" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1003">
-        <v>1</v>
-      </c>
-      <c r="J1003" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1003" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1003">
-        <v>40</v>
-      </c>
-      <c r="M1003" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1004" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1004">
-        <v>22173</v>
-      </c>
-      <c r="B1004" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1004" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1004" s="1">
-        <v>30000</v>
-      </c>
-      <c r="E1004">
-        <v>3</v>
-      </c>
-      <c r="F1004" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1004" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1004" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1004">
-        <v>2</v>
-      </c>
-      <c r="J1004" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1004" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1004">
-        <v>54</v>
-      </c>
-      <c r="M1004" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1005" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1005">
-        <v>12697</v>
-      </c>
-      <c r="B1005" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1005" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1005" s="1">
-        <v>90000</v>
-      </c>
-      <c r="E1005">
-        <v>0</v>
-      </c>
-      <c r="F1005" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1005" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1005" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1005">
-        <v>4</v>
-      </c>
-      <c r="J1005" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1005" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1005">
-        <v>36</v>
-      </c>
-      <c r="M1005" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1006" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1006">
-        <v>11434</v>
-      </c>
-      <c r="B1006" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1006" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1006" s="1">
-        <v>170000</v>
-      </c>
-      <c r="E1006">
-        <v>5</v>
-      </c>
-      <c r="F1006" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1006" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1006" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1006">
-        <v>0</v>
-      </c>
-      <c r="J1006" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1006" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1006">
-        <v>55</v>
-      </c>
-      <c r="M1006" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1007" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1007">
-        <v>25323</v>
-      </c>
-      <c r="B1007" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1007" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1007" s="1">
-        <v>40000</v>
-      </c>
-      <c r="E1007">
-        <v>2</v>
-      </c>
-      <c r="F1007" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1007" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1007" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1007">
-        <v>1</v>
-      </c>
-      <c r="J1007" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1007" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1007">
-        <v>35</v>
-      </c>
-      <c r="M1007" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1008" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1008">
-        <v>23542</v>
-      </c>
-      <c r="B1008" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1008" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1008" s="1">
-        <v>60000</v>
-      </c>
-      <c r="E1008">
-        <v>1</v>
-      </c>
-      <c r="F1008" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1008" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1008" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1008">
-        <v>1</v>
-      </c>
-      <c r="J1008" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1008" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1008">
-        <v>45</v>
-      </c>
-      <c r="M1008" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1009" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1009">
-        <v>20870</v>
-      </c>
-      <c r="B1009" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1009" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1009" s="1">
-        <v>10000</v>
-      </c>
-      <c r="E1009">
-        <v>2</v>
-      </c>
-      <c r="F1009" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1009" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1009" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1009">
-        <v>1</v>
-      </c>
-      <c r="J1009" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1009" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1009">
-        <v>38</v>
-      </c>
-      <c r="M1009" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1010" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1010">
-        <v>23316</v>
-      </c>
-      <c r="B1010" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1010" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1010" s="1">
-        <v>30000</v>
-      </c>
-      <c r="E1010">
-        <v>3</v>
-      </c>
-      <c r="F1010" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1010" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1010" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1010">
-        <v>2</v>
-      </c>
-      <c r="J1010" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1010" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1010">
-        <v>59</v>
-      </c>
-      <c r="M1010" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1011" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1011">
-        <v>12610</v>
-      </c>
-      <c r="B1011" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1011" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1011" s="1">
-        <v>30000</v>
-      </c>
-      <c r="E1011">
-        <v>1</v>
-      </c>
-      <c r="F1011" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1011" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1011" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1011">
-        <v>0</v>
-      </c>
-      <c r="J1011" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1011" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1011">
-        <v>47</v>
-      </c>
-      <c r="M1011" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1012" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1012">
-        <v>27183</v>
-      </c>
-      <c r="B1012" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1012" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1012" s="1">
-        <v>40000</v>
-      </c>
-      <c r="E1012">
-        <v>2</v>
-      </c>
-      <c r="F1012" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1012" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1012" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1012">
-        <v>1</v>
-      </c>
-      <c r="J1012" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1012" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1012">
-        <v>35</v>
-      </c>
-      <c r="M1012" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1013" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1013">
-        <v>25940</v>
-      </c>
-      <c r="B1013" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1013" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1013" s="1">
-        <v>20000</v>
-      </c>
-      <c r="E1013">
-        <v>2</v>
-      </c>
-      <c r="F1013" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1013" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1013" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1013">
-        <v>2</v>
-      </c>
-      <c r="J1013" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1013" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1013">
-        <v>55</v>
-      </c>
-      <c r="M1013" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1014" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1014">
-        <v>25598</v>
-      </c>
-      <c r="B1014" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1014" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1014" s="1">
-        <v>40000</v>
-      </c>
-      <c r="E1014">
-        <v>0</v>
-      </c>
-      <c r="F1014" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1014" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1014" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1014">
-        <v>0</v>
-      </c>
-      <c r="J1014" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1014" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1014">
-        <v>36</v>
-      </c>
-      <c r="M1014" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1015" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1015">
-        <v>21564</v>
-      </c>
-      <c r="B1015" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1015" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1015" s="1">
-        <v>80000</v>
-      </c>
-      <c r="E1015">
-        <v>0</v>
-      </c>
-      <c r="F1015" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1015" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1015" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1015">
-        <v>4</v>
-      </c>
-      <c r="J1015" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1015" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1015">
-        <v>35</v>
-      </c>
-      <c r="M1015" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1016" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1016">
-        <v>19193</v>
-      </c>
-      <c r="B1016" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1016" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1016" s="1">
-        <v>40000</v>
-      </c>
-      <c r="E1016">
-        <v>2</v>
-      </c>
-      <c r="F1016" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1016" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1016" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1016">
-        <v>0</v>
-      </c>
-      <c r="J1016" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1016" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1016">
-        <v>35</v>
-      </c>
-      <c r="M1016" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1017" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1017">
-        <v>26412</v>
-      </c>
-      <c r="B1017" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1017" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1017" s="1">
-        <v>80000</v>
-      </c>
-      <c r="E1017">
-        <v>5</v>
-      </c>
-      <c r="F1017" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1017" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1017" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1017">
-        <v>3</v>
-      </c>
-      <c r="J1017" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1017" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1017">
-        <v>56</v>
-      </c>
-      <c r="M1017" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1018" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1018">
-        <v>27184</v>
-      </c>
-      <c r="B1018" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1018" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1018" s="1">
-        <v>40000</v>
-      </c>
-      <c r="E1018">
-        <v>2</v>
-      </c>
-      <c r="F1018" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1018" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1018" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1018">
-        <v>1</v>
-      </c>
-      <c r="J1018" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1018" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1018">
-        <v>34</v>
-      </c>
-      <c r="M1018" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1019" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1019">
-        <v>12590</v>
-      </c>
-      <c r="B1019" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1019" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1019" s="1">
-        <v>30000</v>
-      </c>
-      <c r="E1019">
-        <v>1</v>
-      </c>
-      <c r="F1019" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1019" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1019" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1019">
-        <v>0</v>
-      </c>
-      <c r="J1019" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1019" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1019">
-        <v>63</v>
-      </c>
-      <c r="M1019" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1020" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1020">
-        <v>17841</v>
-      </c>
-      <c r="B1020" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1020" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1020" s="1">
-        <v>30000</v>
-      </c>
-      <c r="E1020">
-        <v>0</v>
-      </c>
-      <c r="F1020" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1020" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1020" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1020">
-        <v>1</v>
-      </c>
-      <c r="J1020" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1020" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1020">
-        <v>29</v>
-      </c>
-      <c r="M1020" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1021" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1021">
-        <v>18283</v>
-      </c>
-      <c r="B1021" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1021" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1021" s="1">
-        <v>100000</v>
-      </c>
-      <c r="E1021">
-        <v>0</v>
-      </c>
-      <c r="F1021" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1021" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1021" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1021">
-        <v>1</v>
-      </c>
-      <c r="J1021" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1021" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1021">
-        <v>40</v>
-      </c>
-      <c r="M1021" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1022" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1022">
-        <v>18299</v>
-      </c>
-      <c r="B1022" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1022" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1022" s="1">
-        <v>70000</v>
-      </c>
-      <c r="E1022">
-        <v>5</v>
-      </c>
-      <c r="F1022" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1022" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1022" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1022">
-        <v>2</v>
-      </c>
-      <c r="J1022" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1022" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1022">
-        <v>44</v>
-      </c>
-      <c r="M1022" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1023" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1023">
-        <v>16466</v>
-      </c>
-      <c r="B1023" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1023" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1023" s="1">
-        <v>20000</v>
-      </c>
-      <c r="E1023">
-        <v>0</v>
-      </c>
-      <c r="F1023" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1023" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1023" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1023">
-        <v>2</v>
-      </c>
-      <c r="J1023" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1023" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1023">
-        <v>32</v>
-      </c>
-      <c r="M1023" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1024" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1024">
-        <v>19273</v>
-      </c>
-      <c r="B1024" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1024" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1024" s="1">
-        <v>20000</v>
-      </c>
-      <c r="E1024">
-        <v>2</v>
-      </c>
-      <c r="F1024" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1024" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1024" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1024">
-        <v>0</v>
-      </c>
-      <c r="J1024" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1024" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1024">
-        <v>63</v>
-      </c>
-      <c r="M1024" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1025" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1025">
-        <v>22400</v>
-      </c>
-      <c r="B1025" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1025" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1025" s="1">
-        <v>10000</v>
-      </c>
-      <c r="E1025">
-        <v>0</v>
-      </c>
-      <c r="F1025" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1025" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1025" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1025">
-        <v>1</v>
-      </c>
-      <c r="J1025" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1025" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1025">
-        <v>26</v>
-      </c>
-      <c r="M1025" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1026" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1026">
-        <v>20942</v>
-      </c>
-      <c r="B1026" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1026" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1026" s="1">
-        <v>20000</v>
-      </c>
-      <c r="E1026">
-        <v>0</v>
-      </c>
-      <c r="F1026" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1026" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1026" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1026">
-        <v>1</v>
-      </c>
-      <c r="J1026" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1026" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1026">
-        <v>31</v>
-      </c>
-      <c r="M1026" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1027" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1027">
-        <v>18484</v>
-      </c>
-      <c r="B1027" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1027" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1027" s="1">
-        <v>80000</v>
-      </c>
-      <c r="E1027">
-        <v>2</v>
-      </c>
-      <c r="F1027" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1027" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1027" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1027">
-        <v>2</v>
-      </c>
-      <c r="J1027" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1027" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1027">
-        <v>50</v>
-      </c>
-      <c r="M1027" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:M1027" xr:uid="{8E2CB67A-7E7D-470D-BF7C-52E0887E6CCE}"/>
+  <autoFilter ref="A1:M1001" xr:uid="{8E2CB67A-7E7D-470D-BF7C-52E0887E6CCE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>